<commit_message>
Partially complete production data
</commit_message>
<xml_diff>
--- a/Production/UT47.2-ProductionData.xlsx
+++ b/Production/UT47.2-ProductionData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryota\Documents\GitHub\Mir\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E0CAA5-5797-489F-B01C-01BAFE3582FC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41208155-C809-49AB-9560-ABEAE3B13D26}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specification" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
   <si>
     <t>PCB Quantity</t>
   </si>
@@ -120,9 +120,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -130,27 +127,6 @@
   </si>
   <si>
     <t>Y1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>total</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>：</t>
-    </r>
   </si>
   <si>
     <r>
@@ -177,9 +153,6 @@
   </si>
   <si>
     <t>C6</t>
-  </si>
-  <si>
-    <t>C2</t>
   </si>
   <si>
     <r>
@@ -242,12 +215,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>R70</t>
-  </si>
-  <si>
-    <t>R71</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -257,51 +224,27 @@
     <t>Quantity Per PCB</t>
   </si>
   <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>22pF</t>
-  </si>
-  <si>
     <t>SOD-123</t>
   </si>
   <si>
     <t>5.1k</t>
   </si>
   <si>
-    <t>ATmega32U4-AU</t>
-  </si>
-  <si>
     <t>PRTR5V0U2X</t>
   </si>
   <si>
     <t>HRO-TYPE-C-31-M-12</t>
   </si>
   <si>
-    <t>16Mhz</t>
-  </si>
-  <si>
-    <t>C_0805</t>
-  </si>
-  <si>
     <t>D_SOD-123</t>
   </si>
   <si>
     <t>Fuse_SMD1206_Reflow</t>
   </si>
   <si>
-    <t>R_0805</t>
-  </si>
-  <si>
-    <t>TQFP-44_10x10mm_Pitch0.8mm</t>
-  </si>
-  <si>
     <t>SOT143B</t>
   </si>
   <si>
@@ -311,120 +254,27 @@
     <t>Crystal_SMD_3225-4pin_3.2x2.5mm</t>
   </si>
   <si>
-    <t>D1-D70</t>
-  </si>
-  <si>
-    <t>C3, C4, C5</t>
-  </si>
-  <si>
-    <t>C7, C8</t>
-  </si>
-  <si>
-    <t>R67, R68</t>
-  </si>
-  <si>
-    <t>R73, R74</t>
-  </si>
-  <si>
-    <t>Diode, Generic</t>
-  </si>
-  <si>
-    <t>PTC Fuse</t>
-  </si>
-  <si>
-    <t>500mA hold, 1A trip</t>
-  </si>
-  <si>
-    <t>Crystal, 3.2 x 2.5mm, 4 pads</t>
-  </si>
-  <si>
-    <t>USB 2.0 Type-C Connector</t>
-  </si>
-  <si>
-    <t>ESD Protection Diode IC</t>
-  </si>
-  <si>
-    <t>ATMEGA32U4 Microcontroller</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
     <t>Capacitor</t>
   </si>
   <si>
-    <t>Lunar Keyboard PCB</t>
-  </si>
-  <si>
-    <t>478-9926-1-ND</t>
-  </si>
-  <si>
-    <t>1276-2872-1-ND</t>
-  </si>
-  <si>
-    <t>490-4785-1-ND</t>
-  </si>
-  <si>
-    <t>1276-2605-1-ND</t>
-  </si>
-  <si>
-    <t>BAV21W-FDICT-ND</t>
-  </si>
-  <si>
-    <t>F3733CT-ND</t>
-  </si>
-  <si>
-    <t>1253-1698-1-ND‎</t>
-  </si>
-  <si>
     <t>https://lcsc.com/product-detail/USB-Type-C_Korean-Hroparts-Elec-TYPE-C-31-M-12_C165948.html</t>
   </si>
   <si>
-    <t>C165948</t>
-  </si>
-  <si>
-    <t>1727-3884-1-ND</t>
-  </si>
-  <si>
-    <t>ATMEGA32U4-AURCT-ND</t>
-  </si>
-  <si>
-    <t>311-5.10KCRCT-ND</t>
-  </si>
-  <si>
-    <t>311-22.0CRCT-ND</t>
-  </si>
-  <si>
-    <t>RNCP0805FTD1K00CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0805FT10K0CT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>2015010A</t>
-  </si>
-  <si>
-    <t>4060505A</t>
-  </si>
-  <si>
     <t>1/8W Minimum</t>
   </si>
   <si>
     <t>10V Minimum</t>
   </si>
   <si>
-    <t>16V Minimum, X7R</t>
-  </si>
-  <si>
     <t>16V Minimum, C0G</t>
   </si>
   <si>
-    <t>Please see position-bottom.pos</t>
-  </si>
-  <si>
     <t>Please see Layout.pdf</t>
   </si>
   <si>
@@ -435,6 +285,144 @@
   </si>
   <si>
     <t>50pcs</t>
+  </si>
+  <si>
+    <t>Switch sockets in UT47.2-socket.pos</t>
+  </si>
+  <si>
+    <t>Other parts in UT47.2-bottom.pos</t>
+  </si>
+  <si>
+    <t>C_0603</t>
+  </si>
+  <si>
+    <t>MXOnly-1.25U-Hotswap</t>
+  </si>
+  <si>
+    <t>MXOnly-1.5U-Hotswap</t>
+  </si>
+  <si>
+    <t>MXOnly-1U-Hotswap</t>
+  </si>
+  <si>
+    <t>MXOnly-2U-Hotswap-ReversedStabilizers</t>
+  </si>
+  <si>
+    <t>R_0603</t>
+  </si>
+  <si>
+    <t>WS2812B</t>
+  </si>
+  <si>
+    <t>SKQG-1155865</t>
+  </si>
+  <si>
+    <t>QFN-32-1EP_5x5mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>22p</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>500mA</t>
+  </si>
+  <si>
+    <t>MX-1.25U</t>
+  </si>
+  <si>
+    <t>MX-1.5U</t>
+  </si>
+  <si>
+    <t>MX-1U</t>
+  </si>
+  <si>
+    <t>MX-2U</t>
+  </si>
+  <si>
+    <t>SW_PUSH</t>
+  </si>
+  <si>
+    <t>ATMEGA32U2-AU</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>Diode, SOD-123, Generic</t>
+  </si>
+  <si>
+    <t>Kailh MX Hotswap Sockets</t>
+  </si>
+  <si>
+    <t>WS2812B RGB LED, 5050</t>
+  </si>
+  <si>
+    <t>Push button, 5.2 x 5.2mm</t>
+  </si>
+  <si>
+    <t>Atmel ATMEGA32U2, QFN</t>
+  </si>
+  <si>
+    <t>ESD Protection Chip</t>
+  </si>
+  <si>
+    <t>HRO USB connector</t>
+  </si>
+  <si>
+    <t>Crystal, 16MHz, 8-10pF load capacitance, 3.2 x 2.5mm</t>
+  </si>
+  <si>
+    <t>16V Minimum, X5R or X7R</t>
+  </si>
+  <si>
+    <t>Polyfuse, 500mA hold, 1A trip, 1206</t>
+  </si>
+  <si>
+    <t>C4 C5 CR1 CR2 CR3 CR4 CR5 CR6 CR7 CR8</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C1 C2</t>
+  </si>
+  <si>
+    <t>D1 D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47</t>
+  </si>
+  <si>
+    <t>MX13 MX24 MX41 MX43</t>
+  </si>
+  <si>
+    <t>MX12 MX25</t>
+  </si>
+  <si>
+    <t>MX1 MX2 MX3 MX4 MX5 MX6 MX7 MX8 MX9 MX10 MX11 MX14 MX15 MX16 MX17 MX18 MX19 MX20 MX21 MX22 MX23 MX26 MX27 MX28 MX29 MX30 MX31 MX32 MX33 MX34 MX35 MX36 MX37 MX38 MX39 MX40 MX44 MX45 MX46 MX47</t>
+  </si>
+  <si>
+    <t>MX42</t>
+  </si>
+  <si>
+    <t>R1 R5</t>
+  </si>
+  <si>
+    <t>R2 R3</t>
+  </si>
+  <si>
+    <t>R4 R6</t>
+  </si>
+  <si>
+    <t>RGB1 RGB2 RGB3 RGB4 RGB5 RGB6 RGB7 RGB8</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>UT47.2 Keyboard PCB</t>
   </si>
 </sst>
 </file>
@@ -447,6 +435,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -532,13 +527,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -636,70 +624,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -708,34 +693,55 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1092,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1104,10 +1110,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="17"/>
+      <c r="A1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="16"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1117,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1150,7 +1156,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1172,7 +1178,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1183,7 +1189,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1230,22 +1236,22 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
@@ -1272,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1283,35 +1289,35 @@
     <col min="4" max="4" width="20.26953125" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.453125" customWidth="1"/>
-    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="25">
-      <c r="A1" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="A1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="14">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>18</v>
@@ -1341,31 +1347,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" s="4" customFormat="1">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="13">
-        <v>3</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>78</v>
+      <c r="B3" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="21">
+        <v>10</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="H3" s="5">
         <f>(2*C3)</f>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5" t="s">
@@ -1373,71 +1377,65 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A4" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="4" customFormat="1">
+      <c r="A4" s="21">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="B4" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="21">
         <v>1</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>78</v>
+      <c r="D4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H12" si="0">(2*C4)</f>
+        <f t="shared" ref="H4:H15" si="0">(2*C4)</f>
         <v>2</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A5" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="13">
-        <v>1</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>78</v>
+      <c r="B5" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="21">
+        <v>2</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
@@ -1445,34 +1443,32 @@
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A6" s="5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="4" customFormat="1">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="13">
-        <v>2</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>78</v>
+      <c r="B6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5" t="s">
@@ -1480,34 +1476,32 @@
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A7" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="4" customFormat="1">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="13">
-        <v>70</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>70</v>
+      <c r="B7" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="21">
+        <v>47</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
@@ -1516,27 +1510,25 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" s="4" customFormat="1">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="13">
+      <c r="B8" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="21">
         <v>1</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>71</v>
+      <c r="D8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="0"/>
@@ -1546,277 +1538,257 @@
       <c r="J8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1">
+      <c r="A9" s="21">
+        <v>7</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A9" s="5">
-        <v>7</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>77</v>
+      <c r="C9" s="21">
+        <v>4</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" s="5"/>
-      <c r="L9" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A10" s="5">
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1">
+      <c r="A10" s="21">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>77</v>
+      <c r="B10" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" s="5"/>
-      <c r="L10" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A11" s="5">
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1">
+      <c r="A11" s="21">
         <v>9</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="21">
+        <v>40</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="13">
-        <v>2</v>
-      </c>
-      <c r="D11" s="13">
-        <v>22</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>77</v>
+      <c r="F11" s="5"/>
+      <c r="G11" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K11" s="5"/>
-      <c r="L11" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A12" s="5">
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1">
+      <c r="A12" s="21">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="13">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>77</v>
+      <c r="F12" s="5"/>
+      <c r="G12" s="21" t="s">
+        <v>86</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A13" s="5">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1">
+      <c r="A13" s="21">
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>76</v>
+      <c r="B13" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="21">
+        <v>2</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="H13" s="5">
-        <v>44</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A14" s="5">
+      <c r="L13" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1">
+      <c r="A14" s="21">
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="13">
-        <v>1</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>75</v>
+      <c r="B14" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="21">
+        <v>2</v>
+      </c>
+      <c r="D14" s="28">
+        <v>22</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="H14" s="5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" ht="14">
-      <c r="A15" s="5">
+      <c r="L14" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1">
+      <c r="A15" s="21">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="13">
-        <v>1</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>74</v>
+      <c r="B15" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="21">
+        <v>2</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="H15" s="5">
-        <v>12</v>
-      </c>
-      <c r="I15" s="5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A16" s="21">
+        <v>14</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="21">
+        <v>8</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="21" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="5">
-        <v>14</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="H16" s="5">
+        <f>(4 * C16)</f>
         <v>32</v>
-      </c>
-      <c r="C16" s="13">
-        <v>1</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="5">
-        <v>4</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
@@ -1826,88 +1798,160 @@
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" s="4" customFormat="1">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="7">
-        <f>SUM(H3:H16)</f>
-        <v>232</v>
-      </c>
-      <c r="I17" s="7">
-        <f>SUM(I3:I16)</f>
+      <c r="A17" s="21">
+        <v>15</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="21">
+        <v>1</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="5">
         <v>4</v>
       </c>
-      <c r="J17"/>
-      <c r="K17" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" s="4" customFormat="1" ht="15.5">
-      <c r="A18" s="6"/>
-      <c r="B18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" ht="15.5">
-      <c r="A19" s="6"/>
-      <c r="B19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1">
+      <c r="A18" s="21">
+        <v>16</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="21">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="26">
+        <v>32</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+    </row>
+    <row r="19" spans="1:12" s="4" customFormat="1">
+      <c r="A19" s="21">
+        <v>17</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="21">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="23"/>
+      <c r="G19" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="26">
+        <v>4</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
+      <c r="A20" s="21">
+        <v>18</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="21">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="23"/>
+      <c r="G20" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="26">
+        <v>12</v>
+      </c>
+      <c r="I20" s="26">
+        <v>4</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="23"/>
+      <c r="L20" s="15" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
+      <c r="A21" s="21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="26">
+        <v>4</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1">
       <c r="A22"/>
@@ -1917,15 +1961,23 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
+      <c r="H22" s="24">
+        <f>SUM(H3:H21)</f>
+        <v>318</v>
+      </c>
+      <c r="I22" s="24">
+        <f>SUM(I3:I21)</f>
+        <v>4</v>
+      </c>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" s="4" customFormat="1">
+    <row r="23" spans="1:12" s="4" customFormat="1" ht="15.5">
       <c r="A23"/>
-      <c r="B23"/>
+      <c r="B23" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
@@ -1937,9 +1989,11 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" s="4" customFormat="1">
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="15.5">
       <c r="A24"/>
-      <c r="B24"/>
+      <c r="B24" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
@@ -2009,7 +2063,7 @@
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L15" r:id="rId1" xr:uid="{D22DB62E-8EF4-4535-8B47-E750650CBF00}"/>
+    <hyperlink ref="L20" r:id="rId1" xr:uid="{8F393C76-0BEB-40E1-89E0-BA87B8DCBA8D}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId2"/>
@@ -2028,7 +2082,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2097,7 @@
   <dimension ref="A1:F181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -2057,8 +2111,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>102</v>
+      <c r="A1" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2067,7 +2121,9 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="12"/>
+      <c r="A2" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -2075,7 +2131,7 @@
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>

</xml_diff>